<commit_message>
Working version to 1) compute layer dips and 2) computer dip-adjusted depths
</commit_message>
<xml_diff>
--- a/data/water_iso/228_4_wateriso.xlsx
+++ b/data/water_iso/228_4_wateriso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/data/new_structure/water_isotope_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic228_4-detailstudy/github/data/water_iso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220595A7-FB83-4A43-8392-04FA1DE50771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2655491F-D2BA-EB4F-9E46-F61ADEC96B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-800" yWindow="-21100" windowWidth="27640" windowHeight="16940" xr2:uid="{579819F6-CB99-1447-AC9B-6A4A8904F860}"/>
   </bookViews>
@@ -38,141 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>L7</t>
-  </si>
-  <si>
-    <t>L8</t>
-  </si>
-  <si>
-    <t>L9</t>
-  </si>
-  <si>
-    <t>L10</t>
-  </si>
-  <si>
-    <t>L11</t>
-  </si>
-  <si>
-    <t>L12</t>
-  </si>
-  <si>
-    <t>L13</t>
-  </si>
-  <si>
-    <t>L14</t>
-  </si>
-  <si>
-    <t>L15</t>
-  </si>
-  <si>
-    <t>L16</t>
-  </si>
-  <si>
-    <t>L17</t>
-  </si>
-  <si>
-    <t>L18</t>
-  </si>
-  <si>
-    <t>L19</t>
-  </si>
-  <si>
-    <t>L20</t>
-  </si>
-  <si>
-    <t>L21</t>
-  </si>
-  <si>
-    <t>L22</t>
-  </si>
-  <si>
-    <t>L23</t>
-  </si>
-  <si>
-    <t>L24</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -209,88 +74,223 @@
     <t>d</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>C16</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>C24</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>C27</t>
-  </si>
-  <si>
-    <t>C28</t>
+    <t>LISO1</t>
+  </si>
+  <si>
+    <t>LISO2</t>
+  </si>
+  <si>
+    <t>LISO3</t>
+  </si>
+  <si>
+    <t>LISO4</t>
+  </si>
+  <si>
+    <t>LISO5</t>
+  </si>
+  <si>
+    <t>LISO6</t>
+  </si>
+  <si>
+    <t>LISO7</t>
+  </si>
+  <si>
+    <t>LISO8</t>
+  </si>
+  <si>
+    <t>LISO9</t>
+  </si>
+  <si>
+    <t>LISO10</t>
+  </si>
+  <si>
+    <t>LISO11</t>
+  </si>
+  <si>
+    <t>LISO12</t>
+  </si>
+  <si>
+    <t>LISO13</t>
+  </si>
+  <si>
+    <t>LISO14</t>
+  </si>
+  <si>
+    <t>LISO15</t>
+  </si>
+  <si>
+    <t>LISO16</t>
+  </si>
+  <si>
+    <t>LISO17</t>
+  </si>
+  <si>
+    <t>LISO18</t>
+  </si>
+  <si>
+    <t>LISO19</t>
+  </si>
+  <si>
+    <t>LISO20</t>
+  </si>
+  <si>
+    <t>LISO21</t>
+  </si>
+  <si>
+    <t>LISO22</t>
+  </si>
+  <si>
+    <t>LISO23</t>
+  </si>
+  <si>
+    <t>LISO24</t>
+  </si>
+  <si>
+    <t>RISO1</t>
+  </si>
+  <si>
+    <t>RISO2</t>
+  </si>
+  <si>
+    <t>RISO3</t>
+  </si>
+  <si>
+    <t>RISO4</t>
+  </si>
+  <si>
+    <t>RISO5</t>
+  </si>
+  <si>
+    <t>RISO6</t>
+  </si>
+  <si>
+    <t>RISO7</t>
+  </si>
+  <si>
+    <t>RISO8</t>
+  </si>
+  <si>
+    <t>RISO9</t>
+  </si>
+  <si>
+    <t>RISO10</t>
+  </si>
+  <si>
+    <t>RISO11</t>
+  </si>
+  <si>
+    <t>RISO12</t>
+  </si>
+  <si>
+    <t>RISO13</t>
+  </si>
+  <si>
+    <t>RISO14</t>
+  </si>
+  <si>
+    <t>RISO15</t>
+  </si>
+  <si>
+    <t>RISO16</t>
+  </si>
+  <si>
+    <t>RISO17</t>
+  </si>
+  <si>
+    <t>RISO18</t>
+  </si>
+  <si>
+    <t>RISO19</t>
+  </si>
+  <si>
+    <t>RISO20</t>
+  </si>
+  <si>
+    <t>RISO21</t>
+  </si>
+  <si>
+    <t>CISO1</t>
+  </si>
+  <si>
+    <t>CISO2</t>
+  </si>
+  <si>
+    <t>CISO3</t>
+  </si>
+  <si>
+    <t>CISO4</t>
+  </si>
+  <si>
+    <t>CISO5</t>
+  </si>
+  <si>
+    <t>CISO6</t>
+  </si>
+  <si>
+    <t>CISO7</t>
+  </si>
+  <si>
+    <t>CISO8</t>
+  </si>
+  <si>
+    <t>CISO9</t>
+  </si>
+  <si>
+    <t>CISO10</t>
+  </si>
+  <si>
+    <t>CISO11</t>
+  </si>
+  <si>
+    <t>CISO12</t>
+  </si>
+  <si>
+    <t>CISO13</t>
+  </si>
+  <si>
+    <t>CISO14</t>
+  </si>
+  <si>
+    <t>CISO15</t>
+  </si>
+  <si>
+    <t>CISO16</t>
+  </si>
+  <si>
+    <t>CISO17</t>
+  </si>
+  <si>
+    <t>CISO18</t>
+  </si>
+  <si>
+    <t>CISO19</t>
+  </si>
+  <si>
+    <t>CISO20</t>
+  </si>
+  <si>
+    <t>CISO21</t>
+  </si>
+  <si>
+    <t>CISO22</t>
+  </si>
+  <si>
+    <t>CISO23</t>
+  </si>
+  <si>
+    <t>CISO24</t>
+  </si>
+  <si>
+    <t>CISO25</t>
+  </si>
+  <si>
+    <t>CISO26</t>
+  </si>
+  <si>
+    <t>CISO27</t>
+  </si>
+  <si>
+    <t>CISO28</t>
   </si>
 </sst>
 </file>
@@ -367,9 +367,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -407,7 +407,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -513,7 +513,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -655,7 +655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66A5929-8088-494C-B399-C758F1B5C0AC}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47:F74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,42 +676,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <f>155.065+I2/100</f>
@@ -749,7 +749,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B25" si="0">155.065+I3/100</f>
@@ -787,7 +787,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -863,7 +863,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -901,7 +901,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -939,7 +939,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -977,7 +977,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <f>155.065+(I26+1.3)/100</f>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <f t="shared" ref="B27:B46" si="3">155.065+(I27+1.3)/100</f>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <f t="shared" si="3"/>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <f t="shared" si="3"/>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <f t="shared" si="3"/>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <f t="shared" si="3"/>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <f t="shared" si="3"/>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <f t="shared" si="3"/>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <f t="shared" si="3"/>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <f t="shared" si="3"/>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <f t="shared" si="3"/>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B37">
         <f t="shared" si="3"/>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B38">
         <f t="shared" si="3"/>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B39">
         <f t="shared" si="3"/>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B40">
         <f t="shared" si="3"/>
@@ -2173,7 +2173,7 @@
         <v>-292.87</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="G40">
         <v>-36.64</v>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <f t="shared" si="3"/>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B42">
         <f t="shared" si="3"/>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <f t="shared" si="3"/>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B44">
         <f t="shared" si="3"/>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B45">
         <f t="shared" si="3"/>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B46">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
identified a few issues in data
</commit_message>
<xml_diff>
--- a/data/water_iso/228_4_wateriso.xlsx
+++ b/data/water_iso/228_4_wateriso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic228_4-detailstudy/github/data/water_iso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A10FE3-B201-0D45-8496-8649681AF9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C95FE8-6E39-CF4E-93B6-2663CAA249E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-800" yWindow="-21100" windowWidth="27640" windowHeight="16940" xr2:uid="{579819F6-CB99-1447-AC9B-6A4A8904F860}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>mid_depth_relative</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
   <si>
     <t>LISO1</t>
@@ -665,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66A5929-8088-494C-B399-C758F1B5C0AC}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,7 +708,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <f>155.065+I2/100</f>
@@ -749,7 +746,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B25" si="0">155.065+I3/100</f>
@@ -787,7 +784,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
@@ -825,7 +822,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -863,7 +860,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -901,7 +898,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -939,7 +936,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -977,7 +974,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -1015,7 +1012,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -1035,9 +1032,6 @@
       <c r="F10">
         <v>-19.760000000000002</v>
       </c>
-      <c r="G10">
-        <v>-37.22</v>
-      </c>
       <c r="H10">
         <v>3.85</v>
       </c>
@@ -1053,7 +1047,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -1091,7 +1085,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -1129,7 +1123,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -1167,7 +1161,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -1205,7 +1199,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -1243,7 +1237,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -1281,7 +1275,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -1319,7 +1313,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -1357,7 +1351,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -1395,7 +1389,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -1433,7 +1427,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -1471,7 +1465,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -1509,7 +1503,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -1547,7 +1541,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -1585,7 +1579,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -1623,7 +1617,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26">
         <f>155.065+(I26+1.3)/100</f>
@@ -1661,7 +1655,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27">
         <f t="shared" ref="B27:B46" si="3">155.065+(I27+1.3)/100</f>
@@ -1699,7 +1693,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <f t="shared" si="3"/>
@@ -1737,7 +1731,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29">
         <f t="shared" si="3"/>
@@ -1775,7 +1769,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30">
         <f t="shared" si="3"/>
@@ -1813,7 +1807,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <f t="shared" si="3"/>
@@ -1851,7 +1845,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32">
         <f t="shared" si="3"/>
@@ -1889,7 +1883,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33">
         <f t="shared" si="3"/>
@@ -1927,7 +1921,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <f t="shared" si="3"/>
@@ -1965,7 +1959,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <f t="shared" si="3"/>
@@ -2003,7 +1997,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <f t="shared" si="3"/>
@@ -2041,7 +2035,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <f t="shared" si="3"/>
@@ -2079,7 +2073,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <f t="shared" si="3"/>
@@ -2117,7 +2111,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <f t="shared" si="3"/>
@@ -2155,7 +2149,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40">
         <f t="shared" si="3"/>
@@ -2172,9 +2166,6 @@
       <c r="E40">
         <v>-292.87</v>
       </c>
-      <c r="F40" t="s">
-        <v>11</v>
-      </c>
       <c r="G40">
         <v>-36.64</v>
       </c>
@@ -2193,7 +2184,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41">
         <f t="shared" si="3"/>
@@ -2231,7 +2222,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42">
         <f t="shared" si="3"/>
@@ -2269,7 +2260,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <f t="shared" si="3"/>
@@ -2307,7 +2298,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <f t="shared" si="3"/>
@@ -2345,7 +2336,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45">
         <f t="shared" si="3"/>
@@ -2383,7 +2374,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46">
         <f t="shared" si="3"/>
@@ -2421,7 +2412,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" s="2">
         <v>155.07</v>
@@ -2438,7 +2429,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48" s="2">
         <v>155.08000000000001</v>
@@ -2455,7 +2446,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D49" s="2">
         <v>155.09</v>
@@ -2472,7 +2463,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D50" s="2">
         <v>155.1</v>
@@ -2489,7 +2480,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" s="2">
         <v>155.11000000000001</v>
@@ -2506,7 +2497,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D52" s="2">
         <v>155.12</v>
@@ -2523,7 +2514,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="2">
         <v>155.13</v>
@@ -2540,7 +2531,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" s="2">
         <v>155.13999999999999</v>
@@ -2557,7 +2548,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D55" s="2">
         <v>155.15</v>
@@ -2574,7 +2565,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D56" s="2">
         <v>155.16</v>
@@ -2591,7 +2582,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" s="2">
         <v>155.16999999999999</v>
@@ -2608,7 +2599,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D58" s="2">
         <v>155.18</v>
@@ -2625,7 +2616,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D59" s="2">
         <v>155.19</v>
@@ -2642,7 +2633,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D60" s="2">
         <v>155.19999999999999</v>
@@ -2659,7 +2650,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61" s="2">
         <v>155.21</v>
@@ -2676,7 +2667,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D62" s="2">
         <v>155.22</v>
@@ -2693,7 +2684,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D63" s="2">
         <v>155.22999999999999</v>
@@ -2710,7 +2701,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D64" s="2">
         <v>155.24</v>
@@ -2727,7 +2718,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D65" s="2">
         <v>155.25</v>
@@ -2744,7 +2735,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D66" s="2">
         <v>155.26</v>
@@ -2761,7 +2752,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D67" s="2">
         <v>155.27000000000001</v>
@@ -2778,7 +2769,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D68" s="2">
         <v>155.28</v>
@@ -2795,7 +2786,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D69" s="2">
         <v>155.29</v>
@@ -2812,7 +2803,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70" s="2">
         <v>155.30000000000001</v>
@@ -2829,7 +2820,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D71" s="2">
         <v>155.31</v>
@@ -2846,7 +2837,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D72" s="2">
         <v>155.32</v>
@@ -2863,7 +2854,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D73" s="2">
         <v>155.33000000000001</v>
@@ -2880,7 +2871,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D74" s="2">
         <v>155.34</v>

</xml_diff>